<commit_message>
Update cluster and knot info
Update cluster and knot info
</commit_message>
<xml_diff>
--- a/data/KFG_DB_Excel/UR196.xlsx
+++ b/data/KFG_DB_Excel/UR196.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashokkhosla/Desktop/Khipu/fieldguide/data/XLS/ADD_XLSX/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E240C47D-E995-DF40-87B4-5840FB1E14A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3903AA10-143E-6240-93B5-ACE1C0CF0F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="45160" windowHeight="28220" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1928,7 +1928,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L141"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A92" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>